<commit_message>
update docker & change logic crawl data
</commit_message>
<xml_diff>
--- a/server/data/crawled_data.xlsx
+++ b/server/data/crawled_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -22,68 +22,63 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Sườn non chay chiên sả ơt</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxo47ppw2ahcc</t>
-  </si>
-  <si>
-    <t>Ba chỉ nướng  muối ớt</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5ze89j4m9wc8</t>
-  </si>
-  <si>
-    <t>Bò hầm tiêu xanh</t>
-  </si>
-  <si>
-    <t>• Cơm gạo dẻo, nhiều rau xanh • Hộp đựng 4 ngăn đóng gói kĩ • Cơm bao gồm đồ mặn, canh, đồ xào. • Rất vui được ăn trưa cùng bạn.</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr31pkcz14m1da</t>
-  </si>
-  <si>
-    <t>Cá trê chiên mắm xoài</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cơm gạo dẻo, hộp 4 ngăn tiện lợi.
+    <t>Má Đùi gà chiên sốt tiêu đen</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5qnme94k9l6e</t>
+  </si>
+  <si>
+    <t>Thịt kho đậu hũ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
+• Có canh ăn kèm miễn phí
+• Hộp đựng 4 ngăn tiện lợi</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxef49eu3t09d</t>
+  </si>
+  <si>
+    <t>Đậu hũ chiên sốt thịt bằm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
+• Có canh ăn kemf</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5fjziuklnd99</t>
+  </si>
+  <si>
+    <t>Cá nục kho cải chua</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqy2h5xy2oxw51</t>
+  </si>
+  <si>
+    <t>Vịt kho gừng</t>
+  </si>
+  <si>
+    <t>• Cơm gạo dẻo, nhiều rau xanh</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxo3pgolk1wd7</t>
+  </si>
+  <si>
+    <t>Canh chả cá thác lác khổ hoa bào</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30e7y79nyxb7</t>
+  </si>
+  <si>
+    <t>Bánh canh sườn non, trứng cút</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Cá lóc phi lê xé nhỏ ăn kèm chả ram chiên giòn
 • Giá đã bao gồm đủ đồ xào và canh ăn kèm.
 • Rất vui được ăn trưa cùng bạn.</t>
   </si>
   <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30ide8j89lf8</t>
-  </si>
-  <si>
-    <t>Ếch kho tộ</t>
-  </si>
-  <si>
-    <t>Cơm + món mặn + rau xào + canh.</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxgcfqb0ot533</t>
-  </si>
-  <si>
-    <t>Cơm gà Hải Nam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh.
-• Có canh ăn kèm miễn phí.
-• Hộp đựng 4 ngăn tiện lợi.</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxo0nh9jop0e1</t>
-  </si>
-  <si>
-    <t>Heo xào măng</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr38lhwdl39g49</t>
-  </si>
-  <si>
-    <t>Canh khoai sọ hầm xương</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5yt9arw13t58</t>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5zplxvkslgf0</t>
   </si>
   <si>
     <t>Cơm thêm</t>
@@ -495,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -525,26 +520,26 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
@@ -566,15 +561,15 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
@@ -609,27 +604,19 @@
       <c r="A12" t="s">
         <v>27</v>
       </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update readme cho dễ đọc
</commit_message>
<xml_diff>
--- a/server/data/crawled_data.xlsx
+++ b/server/data/crawled_data.xlsx
@@ -13,13 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Image</t>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
   <si>
     <t>Má Đùi gà chiên sốt tiêu đen</t>

</xml_diff>

<commit_message>
feat: build order & menu routes
</commit_message>
<xml_diff>
--- a/server/data/crawled_data.xlsx
+++ b/server/data/crawled_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>title</t>
   </si>
@@ -22,13 +22,36 @@
     <t>image</t>
   </si>
   <si>
-    <t>Má Đùi gà chiên sốt tiêu đen</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5qnme94k9l6e</t>
-  </si>
-  <si>
-    <t>Thịt kho đậu hũ</t>
+    <t>Nấm đùi gà kho măng chay</t>
+  </si>
+  <si>
+    <t>• Cơm gạo dẻo, hộp 4 ngăn tiện lợi. • Giá đã bao gồm đủ đồ xào và canh ăn kèm. • Rất vui được ăn trưa cùng bạn.</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxpsucbvmx0ef</t>
+  </si>
+  <si>
+    <t>Thịt kho mắm ruốc Huế</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Cơm gạo dẻo, hộp 4 ngăn tiện lợi.
+• Giá đã bao gồm đủ đồ xào và canh ăn kèm.
+• Rất vui được ăn trưa cùng bạn.</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2w41lhhz2c30</t>
+  </si>
+  <si>
+    <t>Gà chiên nước mắm</t>
+  </si>
+  <si>
+    <t>Gà chặt cục 200gr/ phânf</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2wwgp8b6ahc2</t>
+  </si>
+  <si>
+    <t>Cá hường chiên sả</t>
   </si>
   <si>
     <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
@@ -36,49 +59,41 @@
 • Hộp đựng 4 ngăn tiện lợi</t>
   </si>
   <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxef49eu3t09d</t>
-  </si>
-  <si>
-    <t>Đậu hũ chiên sốt thịt bằm</t>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2wb66k0n2c07</t>
+  </si>
+  <si>
+    <t>Bò xào cải chua</t>
   </si>
   <si>
     <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
-• Có canh ăn kemf</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5fjziuklnd99</t>
-  </si>
-  <si>
-    <t>Cá nục kho cải chua</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqy2h5xy2oxw51</t>
-  </si>
-  <si>
-    <t>Vịt kho gừng</t>
-  </si>
-  <si>
-    <t>• Cơm gạo dẻo, nhiều rau xanh</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxo3pgolk1wd7</t>
-  </si>
-  <si>
-    <t>Canh chả cá thác lác khổ hoa bào</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30e7y79nyxb7</t>
-  </si>
-  <si>
-    <t>Bánh canh sườn non, trứng cút</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cá lóc phi lê xé nhỏ ăn kèm chả ram chiên giòn
-• Giá đã bao gồm đủ đồ xào và canh ăn kèm.
+• Hộp đựng 4 ngăn tiện lơij</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxogci6p7lw13</t>
+  </si>
+  <si>
+    <t>Cá ngừ kho cà</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqy2xdmbxm10a2</t>
+  </si>
+  <si>
+    <t>Salad ức gà sốt dầu giấm + trứng luộc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
+• Hộp đựng 4 ngăn đóng gói kĩ
+• Cơm bao gồm đồ mặn, canh, đồ xào.
 • Rất vui được ăn trưa cùng bạn.</t>
   </si>
   <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5zplxvkslgf0</t>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxdboro3bfd5b</t>
+  </si>
+  <si>
+    <t>Canh mộc rau củ</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30a204nop0f4</t>
   </si>
   <si>
     <t>Cơm thêm</t>
@@ -490,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -512,111 +527,125 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update order and authentication
</commit_message>
<xml_diff>
--- a/server/data/crawled_data.xlsx
+++ b/server/data/crawled_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>title</t>
   </si>
@@ -22,36 +22,22 @@
     <t>image</t>
   </si>
   <si>
-    <t>Nấm đùi gà kho măng chay</t>
+    <t>Mỳ quảng chay</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr361idjlk7t4b</t>
+  </si>
+  <si>
+    <t>Phile cá chiên sốt teriyaki</t>
   </si>
   <si>
     <t>• Cơm gạo dẻo, hộp 4 ngăn tiện lợi. • Giá đã bao gồm đủ đồ xào và canh ăn kèm. • Rất vui được ăn trưa cùng bạn.</t>
   </si>
   <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxpsucbvmx0ef</t>
-  </si>
-  <si>
-    <t>Thịt kho mắm ruốc Huế</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cơm gạo dẻo, hộp 4 ngăn tiện lợi.
-• Giá đã bao gồm đủ đồ xào và canh ăn kèm.
-• Rất vui được ăn trưa cùng bạn.</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2w41lhhz2c30</t>
-  </si>
-  <si>
-    <t>Gà chiên nước mắm</t>
-  </si>
-  <si>
-    <t>Gà chặt cục 200gr/ phânf</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2wwgp8b6ahc2</t>
-  </si>
-  <si>
-    <t>Cá hường chiên sả</t>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqy3g01uu6ys91</t>
+  </si>
+  <si>
+    <t>Trứng chiên thịt bằm</t>
   </si>
   <si>
     <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
@@ -59,41 +45,46 @@
 • Hộp đựng 4 ngăn tiện lợi</t>
   </si>
   <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2wb66k0n2c07</t>
-  </si>
-  <si>
-    <t>Bò xào cải chua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
-• Hộp đựng 4 ngăn tiện lơij</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxogci6p7lw13</t>
-  </si>
-  <si>
-    <t>Cá ngừ kho cà</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqy2xdmbxm10a2</t>
-  </si>
-  <si>
-    <t>Salad ức gà sốt dầu giấm + trứng luộc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Cơm gạo dẻo, nhiều rau xanh
-• Hộp đựng 4 ngăn đóng gói kĩ
-• Cơm bao gồm đồ mặn, canh, đồ xào.
-• Rất vui được ăn trưa cùng bạn.</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqxdboro3bfd5b</t>
-  </si>
-  <si>
-    <t>Canh mộc rau củ</t>
-  </si>
-  <si>
-    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30a204nop0f4</t>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lqynexwnwz44e1</t>
+  </si>
+  <si>
+    <t>Gà xào bắp non nấm bào ngư</t>
+  </si>
+  <si>
+    <t>Cơm gà chiên ăn kèm cơm, đồ xào, canh</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr30t0ay6z0k75</t>
+  </si>
+  <si>
+    <t>Sườn cốt lết nướng mật ong</t>
+  </si>
+  <si>
+    <t>• Cơm gạo dẻo, nhiều rau xanh. • Có canh ăn kèm miễn phí. • Hộp đựng 4 ngăn tiện dùng.</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr5ynxhsng0418</t>
+  </si>
+  <si>
+    <t>Gà om ớt hiêm</t>
+  </si>
+  <si>
+    <t>Cơm + Đồ mặn + Đồ xào + Canh + Trái cây</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr320g6zmojo64</t>
+  </si>
+  <si>
+    <t>Canh chua cá lóc</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr343zj47jyc01</t>
+  </si>
+  <si>
+    <t>Nui sốt bò bằm</t>
+  </si>
+  <si>
+    <t>https://mms.img.susercontent.com/vn-11134517-7r98o-lr2w1utsrnpg99</t>
   </si>
   <si>
     <t>Cơm thêm</t>
@@ -527,59 +518,59 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
@@ -590,62 +581,59 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>